<commit_message>
Update NREL-118 to newest format
</commit_message>
<xml_diff>
--- a/data/NREL-118/Power_Storage.xlsx
+++ b/data/NREL-118/Power_Storage.xlsx
@@ -650,7 +650,7 @@
       </c>
       <c r="C2" s="4" t="inlineStr">
         <is>
-          <t>v0.0.1</t>
+          <t>v0.0.2</t>
         </is>
       </c>
     </row>
@@ -737,7 +737,7 @@
       </c>
       <c r="Q3" s="5" t="inlineStr">
         <is>
-          <t>IsLDS</t>
+          <t>IsLDES</t>
         </is>
       </c>
       <c r="R3" s="5" t="inlineStr">
@@ -889,7 +889,7 @@
       </c>
       <c r="Q4" s="6" t="inlineStr">
         <is>
-          <t>IsLDS</t>
+          <t>IsLDES</t>
         </is>
       </c>
       <c r="R4" s="6" t="inlineStr">
@@ -1037,7 +1037,7 @@
       </c>
       <c r="Q5" s="7" t="inlineStr">
         <is>
-          <t>Whether the storage unit is a long-duration storage (1) or not (0)</t>
+          <t>Whether the storage unit is a long-duration energy storage (1) or not (0)</t>
         </is>
       </c>
       <c r="R5" s="7" t="inlineStr">

</xml_diff>